<commit_message>
Power BI Flujo proyectos EPC
</commit_message>
<xml_diff>
--- a/data/Project_Accounting/PROYECTOS EPC 2.xlsx
+++ b/data/Project_Accounting/PROYECTOS EPC 2.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://evolticompany.sharepoint.com/sites/EvoltiAdministrativo/Documentos compartidos/Financiero/PROYECTOS/EPC/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AMOSCOSO\Documents\dev\cash_flow_investment_automatization\data\Project_Accounting\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{15856AE3-1D74-4E20-B472-F26300E83FD7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3FF74BC-5F05-46BC-86AE-BAD0B7F48CD3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-103" yWindow="-103" windowWidth="16663" windowHeight="9772" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Hoja1!$A$1:$AA$27</definedName>
@@ -41,10 +42,142 @@
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
+    <author>Moscoso Deossa, Alejandro</author>
     <author>Administrador</author>
   </authors>
   <commentList>
-    <comment ref="H12" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000001000000}">
+    <comment ref="M5" authorId="0" shapeId="0" xr:uid="{B61A8C80-50E8-4986-8719-0F77AB0F999E}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Moscoso Deossa, Alejandro:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+La puse yo, esta estaba en 0</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="S11" authorId="0" shapeId="0" xr:uid="{5FDFD6E8-4884-4B46-BE58-DE0EF9E42B04}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Moscoso Deossa, Alejandro:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Dejen una de las dos 27/06/2025 - 1/07/2025</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="H12" authorId="1" shapeId="0" xr:uid="{00000000-0006-0000-0000-000001000000}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Administrador:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Adicion al Contrato OTRO SI, REFUERZO METALICO $2,750,000</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="K15" authorId="0" shapeId="0" xr:uid="{00510606-631E-4081-8F19-397CD9C259E5}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Moscoso Deossa, Alejandro:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Estan cambiadas las meses/dias
+</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>Administrador</author>
+  </authors>
+  <commentList>
+    <comment ref="F12" authorId="0" shapeId="0" xr:uid="{D94E66AC-F8EF-4A23-A2D3-CB531881F618}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Administrador:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Adicion al Contrato OTRO SI, REFUERZO METALICO $2,750,000</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="G12" authorId="0" shapeId="0" xr:uid="{A78DE303-7C2C-41CE-A164-67C2CCBC5456}">
       <text>
         <r>
           <rPr>
@@ -73,7 +206,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="211" uniqueCount="130">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="254" uniqueCount="127">
   <si>
     <t>TIPO DE PROYECTO</t>
   </si>
@@ -270,9 +403,6 @@
     <t>HOTEL ADAMO(ALEX ALBERTO PAZ HURTADO)</t>
   </si>
   <si>
-    <t>27/06/2025 - 1/07/2025</t>
-  </si>
-  <si>
     <t>2/12/2024-20/02/2025</t>
   </si>
   <si>
@@ -312,9 +442,6 @@
     <t xml:space="preserve">40% A LA FIRMA DEL CONTRATO, 40% ENTREGA DE PANELES E INVERSORES, 20% ENTREGA DE PROYECTO A SATISFACCION </t>
   </si>
   <si>
-    <t>19/12/2024</t>
-  </si>
-  <si>
     <t>EPC-0089</t>
   </si>
   <si>
@@ -322,9 +449,6 @@
   </si>
   <si>
     <t xml:space="preserve">50% A LA FIRMA DE CONTRATO, 40% AL MOMENTO DE INICIAR INSTALACION, 10% ENTREGA DE PROYECTO A SATISFACCION </t>
-  </si>
-  <si>
-    <t>26/12/2024</t>
   </si>
   <si>
     <t xml:space="preserve">PROYECTO NO HA INICIADO DEBIDO A QUE LA PROPIEDAD ESTA EN  CONSTRUCCION </t>
@@ -470,10 +594,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
-    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="164" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="164" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="165" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
-  <fonts count="8">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -530,8 +654,21 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -559,6 +696,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -642,41 +785,41 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="132">
+  <cellXfs count="137">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="43" fontId="2" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="43" fontId="3" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="3" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="14" fontId="4" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="4" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -685,7 +828,7 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -697,16 +840,16 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -754,17 +897,17 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="43" fontId="2" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="2" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="0" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -774,24 +917,24 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="43" fontId="2" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="2" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="164" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="43" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="2" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="2" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -816,13 +959,13 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="43" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="43" fontId="4" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="43" fontId="4" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -846,26 +989,23 @@
     <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="43" fontId="3" fillId="3" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="3" fillId="3" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="14" fontId="4" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="3" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="4" fillId="3" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -873,8 +1013,8 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="43" fontId="2" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="2" fillId="0" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -887,8 +1027,8 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="43" fontId="1" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="43" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="1" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -901,13 +1041,13 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="43" fontId="2" fillId="3" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="2" fillId="3" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="0" fillId="3" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="43" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -919,8 +1059,8 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="43" fontId="2" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="2" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -936,44 +1076,58 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="14" fontId="1" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="43" fontId="1" fillId="5" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="1" fillId="5" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="4" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="5" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="4" fillId="5" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="5" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="0" fillId="5" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="5" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="0" fillId="5" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="5" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="5" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="43" fontId="0" fillId="5" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="14" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="43" fontId="0" fillId="5" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="2" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="4" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="14" fontId="4" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="4" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Millares" xfId="1" builtinId="3"/>
+    <cellStyle name="Comma" xfId="1" builtinId="3"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -994,6 +1148,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1315,40 +1473,44 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AG37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="N2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="X5" sqref="X5"/>
+    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I15" sqref="I15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="14.45"/>
+  <sheetFormatPr defaultColWidth="11.3828125" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
     <col min="1" max="1" width="16" style="28" customWidth="1"/>
     <col min="2" max="2" width="19" style="28" customWidth="1"/>
     <col min="3" max="3" width="21" style="28" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="47" customWidth="1"/>
-    <col min="5" max="5" width="11.85546875" customWidth="1"/>
-    <col min="6" max="6" width="16.140625" style="28" customWidth="1"/>
-    <col min="7" max="7" width="42.140625" customWidth="1"/>
-    <col min="8" max="8" width="23.140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12.42578125" style="123" customWidth="1"/>
-    <col min="10" max="10" width="23.85546875" style="123" customWidth="1"/>
-    <col min="11" max="11" width="12.42578125" customWidth="1"/>
-    <col min="12" max="12" width="20.85546875" style="130" customWidth="1"/>
-    <col min="13" max="13" width="12.42578125" style="1" customWidth="1"/>
-    <col min="14" max="14" width="20.85546875" style="1" customWidth="1"/>
-    <col min="15" max="15" width="15" style="1" customWidth="1"/>
-    <col min="16" max="21" width="14.140625" style="1" customWidth="1"/>
-    <col min="22" max="23" width="15.42578125" style="1" customWidth="1"/>
-    <col min="24" max="24" width="21.85546875" style="1" customWidth="1"/>
-    <col min="25" max="25" width="23.28515625" style="57" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="18.85546875" customWidth="1"/>
-    <col min="27" max="27" width="45.140625" customWidth="1"/>
-    <col min="28" max="28" width="19.7109375" customWidth="1"/>
-    <col min="29" max="29" width="19.140625" customWidth="1"/>
-    <col min="31" max="31" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.84375" customWidth="1"/>
+    <col min="6" max="6" width="16.15234375" style="28" customWidth="1"/>
+    <col min="7" max="7" width="42.15234375" customWidth="1"/>
+    <col min="8" max="8" width="23.15234375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.3828125" style="122" customWidth="1"/>
+    <col min="10" max="10" width="23.84375" style="122" customWidth="1"/>
+    <col min="11" max="11" width="12.3828125" customWidth="1"/>
+    <col min="12" max="12" width="20.84375" style="129" customWidth="1"/>
+    <col min="13" max="13" width="12.3828125" style="134" customWidth="1"/>
+    <col min="14" max="14" width="20.84375" style="1" customWidth="1"/>
+    <col min="15" max="15" width="15" style="134" customWidth="1"/>
+    <col min="16" max="16" width="14.15234375" style="1" customWidth="1"/>
+    <col min="17" max="17" width="14.15234375" style="134" customWidth="1"/>
+    <col min="18" max="18" width="14.15234375" style="1" customWidth="1"/>
+    <col min="19" max="19" width="14.15234375" style="134" customWidth="1"/>
+    <col min="20" max="21" width="14.15234375" style="1" customWidth="1"/>
+    <col min="22" max="23" width="15.3828125" style="1" customWidth="1"/>
+    <col min="24" max="24" width="21.84375" style="1" customWidth="1"/>
+    <col min="25" max="25" width="23.3046875" style="57" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="18.84375" customWidth="1"/>
+    <col min="27" max="27" width="45.15234375" customWidth="1"/>
+    <col min="28" max="28" width="19.69140625" customWidth="1"/>
+    <col min="29" max="29" width="19.15234375" customWidth="1"/>
+    <col min="31" max="31" width="15.3046875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:33" s="60" customFormat="1" ht="49.5" customHeight="1">
+    <row r="1" spans="1:33" s="60" customFormat="1" ht="49.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A1" s="58" t="s">
         <v>0</v>
       </c>
@@ -1373,10 +1535,10 @@
       <c r="H1" s="58" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="111" t="s">
+      <c r="I1" s="110" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="111" t="s">
+      <c r="J1" s="110" t="s">
         <v>9</v>
       </c>
       <c r="K1" s="58" t="s">
@@ -1385,25 +1547,25 @@
       <c r="L1" s="58" t="s">
         <v>10</v>
       </c>
-      <c r="M1" s="58" t="s">
+      <c r="M1" s="132" t="s">
         <v>8</v>
       </c>
       <c r="N1" s="58" t="s">
         <v>10</v>
       </c>
-      <c r="O1" s="58" t="s">
+      <c r="O1" s="132" t="s">
         <v>8</v>
       </c>
       <c r="P1" s="58" t="s">
         <v>10</v>
       </c>
-      <c r="Q1" s="58" t="s">
+      <c r="Q1" s="132" t="s">
         <v>8</v>
       </c>
       <c r="R1" s="58" t="s">
         <v>10</v>
       </c>
-      <c r="S1" s="58" t="s">
+      <c r="S1" s="132" t="s">
         <v>8</v>
       </c>
       <c r="T1" s="58" t="s">
@@ -1431,55 +1593,55 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:33" ht="43.5">
-      <c r="A2" s="88" t="s">
+    <row r="2" spans="1:33" ht="43.75" x14ac:dyDescent="0.4">
+      <c r="A2" s="87" t="s">
         <v>18</v>
       </c>
-      <c r="B2" s="89">
+      <c r="B2" s="88">
         <v>44994</v>
       </c>
-      <c r="C2" s="88" t="s">
+      <c r="C2" s="87" t="s">
         <v>19</v>
       </c>
-      <c r="D2" s="90" t="s">
+      <c r="D2" s="89" t="s">
         <v>20</v>
       </c>
-      <c r="E2" s="91">
+      <c r="E2" s="90">
         <v>71774632</v>
       </c>
-      <c r="F2" s="91" t="s">
+      <c r="F2" s="90" t="s">
         <v>21</v>
       </c>
       <c r="G2" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="H2" s="92">
+      <c r="H2" s="91">
         <v>36000000</v>
       </c>
-      <c r="I2" s="112">
+      <c r="I2" s="111">
         <v>45370</v>
       </c>
-      <c r="J2" s="113">
+      <c r="J2" s="112">
         <v>18000000</v>
       </c>
-      <c r="K2" s="126">
+      <c r="K2" s="125">
         <v>45449</v>
       </c>
-      <c r="L2" s="127">
+      <c r="L2" s="126">
         <v>14400000</v>
       </c>
-      <c r="M2" s="103"/>
-      <c r="N2" s="103"/>
-      <c r="O2" s="103"/>
-      <c r="P2" s="103"/>
-      <c r="Q2" s="103"/>
-      <c r="R2" s="103"/>
-      <c r="S2" s="103"/>
-      <c r="T2" s="103"/>
-      <c r="U2" s="103"/>
-      <c r="V2" s="103"/>
-      <c r="W2" s="103"/>
-      <c r="X2" s="93">
+      <c r="M2" s="102"/>
+      <c r="N2" s="102"/>
+      <c r="O2" s="102"/>
+      <c r="P2" s="102"/>
+      <c r="Q2" s="102"/>
+      <c r="R2" s="102"/>
+      <c r="S2" s="102"/>
+      <c r="T2" s="102"/>
+      <c r="U2" s="102"/>
+      <c r="V2" s="102"/>
+      <c r="W2" s="102"/>
+      <c r="X2" s="92">
         <f>+J2+L2+3600000</f>
         <v>36000000</v>
       </c>
@@ -1487,76 +1649,76 @@
         <f>+H2-X2</f>
         <v>0</v>
       </c>
-      <c r="Z2" s="100" t="s">
+      <c r="Z2" s="99" t="s">
         <v>23</v>
       </c>
       <c r="AA2" s="61" t="s">
         <v>24</v>
       </c>
       <c r="AB2" s="51"/>
-      <c r="AC2" s="101"/>
-      <c r="AD2" s="102"/>
-    </row>
-    <row r="3" spans="1:33" ht="29.1">
-      <c r="A3" s="88" t="s">
+      <c r="AC2" s="100"/>
+      <c r="AD2" s="101"/>
+    </row>
+    <row r="3" spans="1:33" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A3" s="87" t="s">
         <v>18</v>
       </c>
-      <c r="B3" s="89">
+      <c r="B3" s="88">
         <v>45272</v>
       </c>
-      <c r="C3" s="88">
+      <c r="C3" s="87">
         <v>22</v>
       </c>
-      <c r="D3" s="90" t="s">
+      <c r="D3" s="89" t="s">
         <v>25</v>
       </c>
-      <c r="E3" s="104" t="s">
+      <c r="E3" s="103" t="s">
         <v>26</v>
       </c>
-      <c r="F3" s="91" t="s">
+      <c r="F3" s="90" t="s">
         <v>27</v>
       </c>
       <c r="G3" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="H3" s="92">
+      <c r="H3" s="91">
         <v>393822000</v>
       </c>
-      <c r="I3" s="112">
+      <c r="I3" s="111">
         <v>45421</v>
       </c>
-      <c r="J3" s="113">
+      <c r="J3" s="112">
         <v>177219900</v>
       </c>
-      <c r="K3" s="126">
+      <c r="K3" s="125">
         <v>45534</v>
       </c>
-      <c r="L3" s="127">
+      <c r="L3" s="126">
         <v>137837700</v>
       </c>
-      <c r="M3" s="105"/>
-      <c r="N3" s="103"/>
-      <c r="O3" s="105"/>
-      <c r="P3" s="103"/>
-      <c r="Q3" s="105">
+      <c r="M3" s="104"/>
+      <c r="N3" s="102"/>
+      <c r="O3" s="104"/>
+      <c r="P3" s="102"/>
+      <c r="Q3" s="104">
         <v>45649</v>
       </c>
-      <c r="R3" s="106">
+      <c r="R3" s="105">
         <v>61535578</v>
       </c>
-      <c r="S3" s="106"/>
-      <c r="T3" s="106"/>
-      <c r="U3" s="106">
+      <c r="S3" s="105"/>
+      <c r="T3" s="105"/>
+      <c r="U3" s="105">
         <v>6925602.79</v>
       </c>
-      <c r="V3" s="106">
+      <c r="V3" s="105">
         <f>5889455.7+4639729.24+4009559.51</f>
         <v>14538744.450000001</v>
       </c>
-      <c r="W3" s="106">
+      <c r="W3" s="105">
         <v>5800000</v>
       </c>
-      <c r="X3" s="93">
+      <c r="X3" s="92">
         <f>+J3+L3+R3+3815680.34</f>
         <v>380408858.33999997</v>
       </c>
@@ -1564,7 +1726,7 @@
         <f>+H3-X3-V3+U3-W3</f>
         <v>2.514570951461792E-8</v>
       </c>
-      <c r="Z3" s="100" t="s">
+      <c r="Z3" s="99" t="s">
         <v>23</v>
       </c>
       <c r="AA3" s="61" t="s">
@@ -1574,7 +1736,7 @@
       <c r="AC3" s="81"/>
       <c r="AE3" s="51"/>
     </row>
-    <row r="4" spans="1:33" s="5" customFormat="1" ht="84.95" customHeight="1">
+    <row r="4" spans="1:33" s="5" customFormat="1" ht="85" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A4" s="25" t="s">
         <v>18</v>
       </c>
@@ -1599,13 +1761,13 @@
       <c r="H4" s="11">
         <v>1272184759</v>
       </c>
-      <c r="I4" s="114">
+      <c r="I4" s="113">
         <v>45566</v>
       </c>
-      <c r="J4" s="115">
+      <c r="J4" s="114">
         <v>636092380</v>
       </c>
-      <c r="K4" s="128">
+      <c r="K4" s="127">
         <v>45974</v>
       </c>
       <c r="L4" s="21">
@@ -1647,12 +1809,9 @@
       </c>
       <c r="AB4" s="6"/>
       <c r="AC4" s="51"/>
-      <c r="AE4" s="6">
-        <f>+AE3-AB3</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:33" s="42" customFormat="1" ht="82.5" customHeight="1">
+      <c r="AE4" s="6"/>
+    </row>
+    <row r="5" spans="1:33" s="42" customFormat="1" ht="82.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A5" s="25" t="s">
         <v>18</v>
       </c>
@@ -1677,20 +1836,20 @@
       <c r="H5" s="11">
         <v>62097313</v>
       </c>
-      <c r="I5" s="114">
+      <c r="I5" s="113">
         <v>45584</v>
       </c>
-      <c r="J5" s="115">
+      <c r="J5" s="114">
         <v>25000000</v>
       </c>
-      <c r="K5" s="128">
+      <c r="K5" s="127">
         <v>45692</v>
       </c>
       <c r="L5" s="21">
         <v>6048657</v>
       </c>
-      <c r="M5" s="12">
-        <v>0</v>
+      <c r="M5" s="135">
+        <v>45688</v>
       </c>
       <c r="N5" s="13">
         <v>5000000</v>
@@ -1727,7 +1886,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="6" spans="1:33" s="42" customFormat="1" ht="56.1" customHeight="1">
+    <row r="6" spans="1:33" s="42" customFormat="1" ht="56.15" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A6" s="25" t="s">
         <v>18</v>
       </c>
@@ -1752,13 +1911,13 @@
       <c r="H6" s="11">
         <v>100783942</v>
       </c>
-      <c r="I6" s="114">
+      <c r="I6" s="113">
         <v>45635</v>
       </c>
-      <c r="J6" s="115">
+      <c r="J6" s="114">
         <v>50391971</v>
       </c>
-      <c r="K6" s="128">
+      <c r="K6" s="127">
         <v>45799</v>
       </c>
       <c r="L6" s="21">
@@ -1797,7 +1956,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="7" spans="1:33" s="5" customFormat="1" ht="48.6" customHeight="1">
+    <row r="7" spans="1:33" s="5" customFormat="1" ht="48.65" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A7" s="25" t="s">
         <v>18</v>
       </c>
@@ -1822,13 +1981,13 @@
       <c r="H7" s="11">
         <v>81223400</v>
       </c>
-      <c r="I7" s="114">
+      <c r="I7" s="113">
         <v>45582</v>
       </c>
-      <c r="J7" s="115">
+      <c r="J7" s="114">
         <v>78705475</v>
       </c>
-      <c r="K7" s="128"/>
+      <c r="K7" s="127"/>
       <c r="L7" s="21">
         <v>0</v>
       </c>
@@ -1864,7 +2023,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="8" spans="1:33" s="5" customFormat="1" ht="87.6" customHeight="1">
+    <row r="8" spans="1:33" s="5" customFormat="1" ht="87.65" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="29" t="s">
         <v>18</v>
       </c>
@@ -1889,13 +2048,13 @@
       <c r="H8" s="20">
         <v>620027595</v>
       </c>
-      <c r="I8" s="114">
+      <c r="I8" s="113">
         <v>45707</v>
       </c>
-      <c r="J8" s="115">
+      <c r="J8" s="114">
         <v>248011038</v>
       </c>
-      <c r="K8" s="128"/>
+      <c r="K8" s="127"/>
       <c r="L8" s="21"/>
       <c r="M8" s="21">
         <v>0</v>
@@ -1927,7 +2086,7 @@
       <c r="AC8" s="81"/>
       <c r="AE8" s="6"/>
     </row>
-    <row r="9" spans="1:33" s="5" customFormat="1" ht="94.5" customHeight="1">
+    <row r="9" spans="1:33" s="5" customFormat="1" ht="94.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A9" s="25" t="s">
         <v>18</v>
       </c>
@@ -1952,13 +2111,13 @@
       <c r="H9" s="11">
         <v>26902449</v>
       </c>
-      <c r="I9" s="114">
+      <c r="I9" s="113">
         <v>45608</v>
       </c>
-      <c r="J9" s="115">
+      <c r="J9" s="114">
         <v>13451225</v>
       </c>
-      <c r="K9" s="128">
+      <c r="K9" s="127">
         <v>45698</v>
       </c>
       <c r="L9" s="21">
@@ -1970,7 +2129,7 @@
       </c>
       <c r="O9" s="13"/>
       <c r="P9" s="13"/>
-      <c r="Q9" s="13">
+      <c r="Q9" s="133">
         <v>45761</v>
       </c>
       <c r="R9" s="13">
@@ -2001,7 +2160,7 @@
       <c r="AE9" s="22"/>
       <c r="AG9" s="22"/>
     </row>
-    <row r="10" spans="1:33" s="5" customFormat="1" ht="105.95" customHeight="1">
+    <row r="10" spans="1:33" s="5" customFormat="1" ht="106" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="70" t="s">
         <v>18</v>
       </c>
@@ -2026,13 +2185,13 @@
       <c r="H10" s="75">
         <v>73268018</v>
       </c>
-      <c r="I10" s="114">
+      <c r="I10" s="113">
         <v>45587</v>
       </c>
-      <c r="J10" s="115">
+      <c r="J10" s="114">
         <v>7326802</v>
       </c>
-      <c r="K10" s="128">
+      <c r="K10" s="127">
         <v>45650</v>
       </c>
       <c r="L10" s="21">
@@ -2077,7 +2236,7 @@
       <c r="AC10" s="81"/>
       <c r="AE10" s="6"/>
     </row>
-    <row r="11" spans="1:33" s="5" customFormat="1" ht="84" customHeight="1">
+    <row r="11" spans="1:33" s="5" customFormat="1" ht="84" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A11" s="25" t="s">
         <v>18</v>
       </c>
@@ -2102,13 +2261,13 @@
       <c r="H11" s="11">
         <v>65541486</v>
       </c>
-      <c r="I11" s="114">
+      <c r="I11" s="113">
         <v>45618</v>
       </c>
-      <c r="J11" s="115">
+      <c r="J11" s="114">
         <v>25000000</v>
       </c>
-      <c r="K11" s="128">
+      <c r="K11" s="127">
         <v>45631</v>
       </c>
       <c r="L11" s="21">
@@ -2132,8 +2291,8 @@
       <c r="R11" s="13">
         <v>6000000</v>
       </c>
-      <c r="S11" s="82" t="s">
-        <v>65</v>
+      <c r="S11" s="136">
+        <v>45839</v>
       </c>
       <c r="T11" s="13">
         <f>12100000+1224891</f>
@@ -2153,22 +2312,22 @@
       <c r="Z11" s="52" t="s">
         <v>23</v>
       </c>
-      <c r="AA11" s="107" t="s">
+      <c r="AA11" s="106" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="12" spans="1:33" s="5" customFormat="1" ht="77.45" customHeight="1">
+    <row r="12" spans="1:33" s="5" customFormat="1" ht="77.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A12" s="70" t="s">
         <v>18</v>
       </c>
       <c r="B12" s="71" t="s">
+        <v>65</v>
+      </c>
+      <c r="C12" s="70" t="s">
         <v>66</v>
       </c>
-      <c r="C12" s="70" t="s">
+      <c r="D12" s="72" t="s">
         <v>67</v>
-      </c>
-      <c r="D12" s="72" t="s">
-        <v>68</v>
       </c>
       <c r="E12" s="72">
         <v>37082297</v>
@@ -2183,13 +2342,13 @@
         <f>57526407+2750000</f>
         <v>60276407</v>
       </c>
-      <c r="I12" s="114">
+      <c r="I12" s="113">
         <v>45628</v>
       </c>
-      <c r="J12" s="115">
+      <c r="J12" s="114">
         <v>28763204</v>
       </c>
-      <c r="K12" s="128">
+      <c r="K12" s="127">
         <v>45653</v>
       </c>
       <c r="L12" s="21">
@@ -2220,11 +2379,11 @@
         <v>23</v>
       </c>
       <c r="AA12" s="65" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="AC12" s="6"/>
     </row>
-    <row r="13" spans="1:33" s="5" customFormat="1" ht="113.1" customHeight="1">
+    <row r="13" spans="1:33" s="5" customFormat="1" ht="113.15" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A13" s="29" t="s">
         <v>18</v>
       </c>
@@ -2232,30 +2391,30 @@
         <v>45639</v>
       </c>
       <c r="C13" s="29" t="s">
+        <v>69</v>
+      </c>
+      <c r="D13" s="18" t="s">
         <v>70</v>
       </c>
-      <c r="D13" s="18" t="s">
+      <c r="E13" s="19" t="s">
         <v>71</v>
-      </c>
-      <c r="E13" s="19" t="s">
-        <v>72</v>
       </c>
       <c r="F13" s="24" t="s">
         <v>33</v>
       </c>
       <c r="G13" s="18" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="H13" s="20">
         <v>239832910</v>
       </c>
-      <c r="I13" s="114">
+      <c r="I13" s="113">
         <v>45747</v>
       </c>
-      <c r="J13" s="115">
+      <c r="J13" s="114">
         <v>95933163</v>
       </c>
-      <c r="K13" s="128"/>
+      <c r="K13" s="127"/>
       <c r="L13" s="21">
         <v>0</v>
       </c>
@@ -2284,12 +2443,12 @@
       </c>
       <c r="Z13" s="52"/>
       <c r="AA13" s="64" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="AB13" s="43"/>
       <c r="AC13" s="6"/>
     </row>
-    <row r="14" spans="1:33" s="17" customFormat="1" ht="47.1" customHeight="1">
+    <row r="14" spans="1:33" s="17" customFormat="1" ht="47.15" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A14" s="34" t="s">
         <v>18</v>
       </c>
@@ -2297,27 +2456,27 @@
         <v>45602</v>
       </c>
       <c r="C14" s="34" t="s">
+        <v>74</v>
+      </c>
+      <c r="D14" s="38" t="s">
         <v>75</v>
       </c>
-      <c r="D14" s="38" t="s">
+      <c r="E14" s="36" t="s">
         <v>76</v>
-      </c>
-      <c r="E14" s="36" t="s">
-        <v>77</v>
       </c>
       <c r="F14" s="37" t="s">
         <v>43</v>
       </c>
       <c r="G14" s="38" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="H14" s="39">
         <v>279034822</v>
       </c>
-      <c r="I14" s="116" t="s">
-        <v>79</v>
-      </c>
-      <c r="J14" s="124">
+      <c r="I14" s="115">
+        <v>45645</v>
+      </c>
+      <c r="J14" s="123">
         <f>+H14*40%</f>
         <v>111613928.80000001</v>
       </c>
@@ -2357,7 +2516,7 @@
       </c>
       <c r="AC14" s="80"/>
     </row>
-    <row r="15" spans="1:33" s="17" customFormat="1" ht="85.5" customHeight="1">
+    <row r="15" spans="1:33" s="17" customFormat="1" ht="85.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A15" s="30" t="s">
         <v>18</v>
       </c>
@@ -2365,10 +2524,10 @@
         <v>45649</v>
       </c>
       <c r="C15" s="30" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="E15" s="3">
         <v>12957938</v>
@@ -2377,20 +2536,20 @@
         <v>33</v>
       </c>
       <c r="G15" s="2" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="H15" s="4">
         <v>77736480</v>
       </c>
-      <c r="I15" s="116">
+      <c r="I15" s="115">
         <v>45652</v>
       </c>
-      <c r="J15" s="117">
+      <c r="J15" s="116">
         <f>+H15*50%</f>
         <v>38868240</v>
       </c>
-      <c r="K15" s="15" t="s">
-        <v>83</v>
+      <c r="K15" s="15">
+        <v>45652</v>
       </c>
       <c r="L15" s="16">
         <v>0</v>
@@ -2420,10 +2579,10 @@
       </c>
       <c r="Z15" s="53"/>
       <c r="AA15" s="68" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="16" spans="1:33" s="17" customFormat="1" ht="63.95" customHeight="1">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="16" spans="1:33" s="17" customFormat="1" ht="64" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A16" s="34" t="s">
         <v>18</v>
       </c>
@@ -2431,27 +2590,27 @@
         <v>45652</v>
       </c>
       <c r="C16" s="34" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="D16" s="38" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="E16" s="36" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="F16" s="37" t="s">
         <v>33</v>
       </c>
       <c r="G16" s="38" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="H16" s="39">
         <v>62633204</v>
       </c>
-      <c r="I16" s="116">
+      <c r="I16" s="115">
         <v>45653</v>
       </c>
-      <c r="J16" s="117">
+      <c r="J16" s="116">
         <v>12526641</v>
       </c>
       <c r="K16" s="15">
@@ -2492,7 +2651,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="17" spans="1:27" s="17" customFormat="1" ht="55.5" customHeight="1">
+    <row r="17" spans="1:27" s="17" customFormat="1" ht="55.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A17" s="30" t="s">
         <v>18</v>
       </c>
@@ -2500,10 +2659,10 @@
         <v>45643</v>
       </c>
       <c r="C17" s="30" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="E17" s="3">
         <v>16359436</v>
@@ -2512,15 +2671,15 @@
         <v>43</v>
       </c>
       <c r="G17" s="2" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="H17" s="4">
         <v>252823862</v>
       </c>
-      <c r="I17" s="116">
+      <c r="I17" s="115">
         <v>45728</v>
       </c>
-      <c r="J17" s="117">
+      <c r="J17" s="116">
         <v>126411931</v>
       </c>
       <c r="K17" s="15"/>
@@ -2552,10 +2711,10 @@
       </c>
       <c r="Z17" s="53"/>
       <c r="AA17" s="69" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="18" spans="1:27" ht="109.5" customHeight="1">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="18" spans="1:27" ht="109.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A18" s="30" t="s">
         <v>18</v>
       </c>
@@ -2563,27 +2722,27 @@
         <v>45326</v>
       </c>
       <c r="C18" s="30" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="E18" s="3">
         <v>1144055891</v>
       </c>
       <c r="F18" s="27" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="G18" s="2" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="H18" s="4">
         <v>28500000</v>
       </c>
-      <c r="I18" s="125">
+      <c r="I18" s="124">
         <v>45691</v>
       </c>
-      <c r="J18" s="118">
+      <c r="J18" s="117">
         <v>5000000</v>
       </c>
       <c r="K18" s="15">
@@ -2617,55 +2776,55 @@
       </c>
       <c r="Z18" s="53"/>
       <c r="AA18" s="7" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="19" spans="1:27" ht="72.900000000000006" x14ac:dyDescent="0.4">
+      <c r="A19" s="93" t="s">
+        <v>18</v>
+      </c>
+      <c r="B19" s="94">
+        <v>45688</v>
+      </c>
+      <c r="C19" s="93" t="s">
+        <v>94</v>
+      </c>
+      <c r="D19" s="95" t="s">
+        <v>95</v>
+      </c>
+      <c r="E19" s="108" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="19" spans="1:27" ht="72.599999999999994">
-      <c r="A19" s="94" t="s">
-        <v>18</v>
-      </c>
-      <c r="B19" s="95">
-        <v>45688</v>
-      </c>
-      <c r="C19" s="94" t="s">
-        <v>97</v>
-      </c>
-      <c r="D19" s="96" t="s">
-        <v>98</v>
-      </c>
-      <c r="E19" s="109" t="s">
-        <v>99</v>
-      </c>
-      <c r="F19" s="97" t="s">
+      <c r="F19" s="96" t="s">
         <v>43</v>
       </c>
-      <c r="G19" s="96" t="s">
-        <v>88</v>
-      </c>
-      <c r="H19" s="98">
+      <c r="G19" s="95" t="s">
+        <v>85</v>
+      </c>
+      <c r="H19" s="97">
         <v>212400000</v>
       </c>
-      <c r="I19" s="125">
+      <c r="I19" s="124">
         <v>45771</v>
       </c>
-      <c r="J19" s="118">
+      <c r="J19" s="117">
         <f>+H19/2</f>
         <v>106200000</v>
       </c>
       <c r="K19" s="15"/>
       <c r="L19" s="23"/>
-      <c r="M19" s="110"/>
-      <c r="N19" s="99"/>
-      <c r="O19" s="99"/>
-      <c r="P19" s="99"/>
-      <c r="Q19" s="99"/>
-      <c r="R19" s="99"/>
-      <c r="S19" s="99"/>
-      <c r="T19" s="99"/>
-      <c r="U19" s="99"/>
-      <c r="V19" s="99"/>
-      <c r="W19" s="99"/>
-      <c r="X19" s="99">
+      <c r="M19" s="109"/>
+      <c r="N19" s="98"/>
+      <c r="O19" s="98"/>
+      <c r="P19" s="98"/>
+      <c r="Q19" s="98"/>
+      <c r="R19" s="98"/>
+      <c r="S19" s="98"/>
+      <c r="T19" s="98"/>
+      <c r="U19" s="98"/>
+      <c r="V19" s="98"/>
+      <c r="W19" s="98"/>
+      <c r="X19" s="98">
         <f>+J19</f>
         <v>106200000</v>
       </c>
@@ -2676,11 +2835,11 @@
       <c r="Z19" s="53" t="s">
         <v>23</v>
       </c>
-      <c r="AA19" s="108" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="20" spans="1:27" ht="59.45" customHeight="1">
+      <c r="AA19" s="107" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="20" spans="1:27" ht="59.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A20" s="30" t="s">
         <v>18</v>
       </c>
@@ -2688,25 +2847,25 @@
         <v>45743</v>
       </c>
       <c r="C20" s="30" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="D20" s="79" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="E20" s="3" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="F20" s="27" t="s">
         <v>33</v>
       </c>
       <c r="G20" s="2" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="H20" s="48">
         <v>149513940</v>
       </c>
-      <c r="I20" s="121"/>
-      <c r="J20" s="119"/>
+      <c r="I20" s="120"/>
+      <c r="J20" s="118"/>
       <c r="K20" s="7"/>
       <c r="L20" s="49"/>
       <c r="M20" s="50"/>
@@ -2730,10 +2889,10 @@
       </c>
       <c r="Z20" s="7"/>
       <c r="AA20" s="7" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="21" spans="1:27" ht="81" customHeight="1">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="21" spans="1:27" ht="81" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A21" s="30" t="s">
         <v>18</v>
       </c>
@@ -2741,27 +2900,27 @@
         <v>45743</v>
       </c>
       <c r="C21" s="30" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="E21" s="3" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="F21" s="27" t="s">
         <v>33</v>
       </c>
       <c r="G21" s="2" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="H21" s="4">
         <v>50550000</v>
       </c>
-      <c r="I21" s="121">
+      <c r="I21" s="120">
         <v>45868</v>
       </c>
-      <c r="J21" s="131">
+      <c r="J21" s="130">
         <v>25275000</v>
       </c>
       <c r="K21" s="7"/>
@@ -2787,10 +2946,10 @@
       </c>
       <c r="Z21" s="7"/>
       <c r="AA21" s="7" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="22" spans="1:27" ht="43.5">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="22" spans="1:27" ht="43.75" x14ac:dyDescent="0.4">
       <c r="A22" s="30" t="s">
         <v>18</v>
       </c>
@@ -2798,27 +2957,27 @@
         <v>45763</v>
       </c>
       <c r="C22" s="30" t="s">
+        <v>105</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="E22" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="F22" s="27" t="s">
+        <v>91</v>
+      </c>
+      <c r="G22" s="2" t="s">
         <v>108</v>
-      </c>
-      <c r="D22" s="2" t="s">
-        <v>109</v>
-      </c>
-      <c r="E22" s="3" t="s">
-        <v>110</v>
-      </c>
-      <c r="F22" s="27" t="s">
-        <v>94</v>
-      </c>
-      <c r="G22" s="2" t="s">
-        <v>111</v>
       </c>
       <c r="H22" s="4">
         <v>65000000</v>
       </c>
-      <c r="I22" s="121">
+      <c r="I22" s="120">
         <v>45772</v>
       </c>
-      <c r="J22" s="120">
+      <c r="J22" s="119">
         <v>39000000</v>
       </c>
       <c r="K22" s="50">
@@ -2848,10 +3007,10 @@
       </c>
       <c r="Z22" s="7"/>
       <c r="AA22" s="7" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="23" spans="1:27" ht="43.5">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="23" spans="1:27" ht="43.75" x14ac:dyDescent="0.4">
       <c r="A23" s="44" t="s">
         <v>18</v>
       </c>
@@ -2859,27 +3018,27 @@
         <v>45771</v>
       </c>
       <c r="C23" s="44" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="E23" s="3" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="F23" s="44" t="s">
         <v>33</v>
       </c>
       <c r="G23" s="2" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="H23" s="4">
         <v>106183000</v>
       </c>
-      <c r="I23" s="121">
+      <c r="I23" s="120">
         <v>45833</v>
       </c>
-      <c r="J23" s="120">
+      <c r="J23" s="119">
         <v>63709800</v>
       </c>
       <c r="K23" s="7"/>
@@ -2905,10 +3064,10 @@
       </c>
       <c r="Z23" s="7"/>
       <c r="AA23" s="61" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="24" spans="1:27" ht="57.95">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="24" spans="1:27" ht="58.3" x14ac:dyDescent="0.4">
       <c r="A24" s="44" t="s">
         <v>18</v>
       </c>
@@ -2916,26 +3075,26 @@
         <v>45797</v>
       </c>
       <c r="C24" s="44" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="E24" s="3" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="F24" s="44" t="s">
         <v>43</v>
       </c>
       <c r="G24" s="2" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="H24" s="4">
         <f>363610000+12000000+11006866</f>
         <v>386616866</v>
       </c>
-      <c r="I24" s="119"/>
-      <c r="J24" s="119"/>
+      <c r="I24" s="118"/>
+      <c r="J24" s="118"/>
       <c r="K24" s="7"/>
       <c r="L24" s="49"/>
       <c r="M24" s="8"/>
@@ -2956,10 +3115,10 @@
       </c>
       <c r="Z24" s="7"/>
       <c r="AA24" s="61" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="25" spans="1:27" ht="57.95">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="25" spans="1:27" ht="58.3" x14ac:dyDescent="0.4">
       <c r="A25" s="44" t="s">
         <v>18</v>
       </c>
@@ -2967,25 +3126,25 @@
         <v>45812</v>
       </c>
       <c r="C25" s="44" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="E25" s="3" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="F25" s="44" t="s">
         <v>33</v>
       </c>
       <c r="G25" s="2" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="H25" s="4">
         <v>669683741</v>
       </c>
-      <c r="I25" s="119"/>
-      <c r="J25" s="119"/>
+      <c r="I25" s="118"/>
+      <c r="J25" s="118"/>
       <c r="K25" s="7"/>
       <c r="L25" s="49"/>
       <c r="M25" s="8"/>
@@ -3007,7 +3166,7 @@
       <c r="Z25" s="7"/>
       <c r="AA25" s="61"/>
     </row>
-    <row r="26" spans="1:27" ht="29.1">
+    <row r="26" spans="1:27" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A26" s="44" t="s">
         <v>18</v>
       </c>
@@ -3015,25 +3174,25 @@
         <v>45799</v>
       </c>
       <c r="C26" s="44" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="E26" s="3"/>
       <c r="F26" s="44" t="s">
         <v>33</v>
       </c>
       <c r="G26" s="2" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="H26" s="4">
         <v>32528526</v>
       </c>
-      <c r="I26" s="121">
+      <c r="I26" s="120">
         <v>45860</v>
       </c>
-      <c r="J26" s="131">
+      <c r="J26" s="130">
         <v>9758558</v>
       </c>
       <c r="K26" s="7"/>
@@ -3059,24 +3218,24 @@
       </c>
       <c r="Z26" s="7"/>
       <c r="AA26" s="61" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="27" spans="1:27">
-      <c r="A27" s="83" t="s">
-        <v>129</v>
-      </c>
-      <c r="B27" s="84"/>
-      <c r="C27" s="84"/>
-      <c r="D27" s="85"/>
+        <v>125</v>
+      </c>
+    </row>
+    <row r="27" spans="1:27" x14ac:dyDescent="0.4">
+      <c r="A27" s="82" t="s">
+        <v>126</v>
+      </c>
+      <c r="B27" s="83"/>
+      <c r="C27" s="83"/>
+      <c r="D27" s="84"/>
       <c r="E27" s="46"/>
-      <c r="F27" s="84"/>
-      <c r="G27" s="85"/>
-      <c r="H27" s="85"/>
-      <c r="I27" s="122"/>
-      <c r="J27" s="122"/>
+      <c r="F27" s="83"/>
+      <c r="G27" s="84"/>
+      <c r="H27" s="84"/>
+      <c r="I27" s="121"/>
+      <c r="J27" s="121"/>
       <c r="K27" s="46"/>
-      <c r="L27" s="129"/>
+      <c r="L27" s="128"/>
       <c r="M27" s="47"/>
       <c r="N27" s="47"/>
       <c r="O27" s="47"/>
@@ -3088,48 +3247,725 @@
       <c r="U27" s="47"/>
       <c r="V27" s="47"/>
       <c r="W27" s="47"/>
-      <c r="X27" s="86"/>
-      <c r="Y27" s="87">
+      <c r="X27" s="85"/>
+      <c r="Y27" s="86">
         <f>SUM(Y2:Y26)</f>
         <v>2107722241.8759999</v>
       </c>
     </row>
-    <row r="29" spans="1:27">
+    <row r="29" spans="1:27" x14ac:dyDescent="0.4">
       <c r="H29" s="78"/>
     </row>
-    <row r="30" spans="1:27">
+    <row r="30" spans="1:27" x14ac:dyDescent="0.4">
       <c r="H30" s="78"/>
     </row>
-    <row r="31" spans="1:27">
+    <row r="31" spans="1:27" x14ac:dyDescent="0.4">
       <c r="H31" s="78"/>
     </row>
-    <row r="32" spans="1:27">
+    <row r="32" spans="1:27" x14ac:dyDescent="0.4">
       <c r="H32" s="78"/>
     </row>
-    <row r="34" spans="8:8">
+    <row r="34" spans="8:8" x14ac:dyDescent="0.4">
       <c r="H34" s="51"/>
     </row>
-    <row r="37" spans="8:8">
+    <row r="37" spans="8:8" x14ac:dyDescent="0.4">
       <c r="H37" s="51"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:AA27" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
   <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
 
-<file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F3E3458D-F684-4410-80D6-E7206E631A4D}">
+  <dimension ref="A1:M37"/>
+  <sheetViews>
+    <sheetView topLeftCell="C1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="L15" sqref="L15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <cols>
+    <col min="1" max="1" width="47" customWidth="1"/>
+    <col min="4" max="4" width="11.84375" customWidth="1"/>
+    <col min="6" max="7" width="23.15234375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="19" style="28" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A1" s="58" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" s="58" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="58" t="s">
+        <v>7</v>
+      </c>
+      <c r="G1" s="58" t="s">
+        <v>7</v>
+      </c>
+      <c r="K1" s="58" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A2" s="89" t="s">
+        <v>20</v>
+      </c>
+      <c r="D2" s="90">
+        <v>71774632</v>
+      </c>
+      <c r="F2" s="91">
+        <v>36000000</v>
+      </c>
+      <c r="G2" s="91">
+        <v>36000000</v>
+      </c>
+      <c r="K2" s="88">
+        <v>44994</v>
+      </c>
+      <c r="L2">
+        <f>+YEAR(K2)</f>
+        <v>2023</v>
+      </c>
+      <c r="M2">
+        <f>+MONTH(K2)</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A3" s="89" t="s">
+        <v>25</v>
+      </c>
+      <c r="D3" s="103" t="s">
+        <v>26</v>
+      </c>
+      <c r="F3" s="91">
+        <v>393822000</v>
+      </c>
+      <c r="G3" s="91">
+        <v>393822000</v>
+      </c>
+      <c r="K3" s="88">
+        <v>45272</v>
+      </c>
+      <c r="L3">
+        <f t="shared" ref="L3:L26" si="0">+YEAR(K3)</f>
+        <v>2023</v>
+      </c>
+      <c r="M3">
+        <f t="shared" ref="M3:M26" si="1">+MONTH(K3)</f>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A4" s="14" t="s">
+        <v>31</v>
+      </c>
+      <c r="D4" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="F4" s="11">
+        <v>1272184759</v>
+      </c>
+      <c r="G4" s="11">
+        <v>1272184759</v>
+      </c>
+      <c r="K4" s="32">
+        <v>45551</v>
+      </c>
+      <c r="L4">
+        <f t="shared" si="0"/>
+        <v>2024</v>
+      </c>
+      <c r="M4">
+        <f t="shared" si="1"/>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A5" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="D5" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="F5" s="11">
+        <v>62097313</v>
+      </c>
+      <c r="G5" s="11">
+        <v>62097313</v>
+      </c>
+      <c r="K5" s="32">
+        <v>45572</v>
+      </c>
+      <c r="L5">
+        <f t="shared" si="0"/>
+        <v>2024</v>
+      </c>
+      <c r="M5">
+        <f t="shared" si="1"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A6" s="14" t="s">
+        <v>41</v>
+      </c>
+      <c r="D6" s="14" t="s">
+        <v>42</v>
+      </c>
+      <c r="F6" s="11">
+        <v>100783942</v>
+      </c>
+      <c r="G6" s="11">
+        <v>100783942</v>
+      </c>
+      <c r="K6" s="32">
+        <v>45575</v>
+      </c>
+      <c r="L6">
+        <f t="shared" si="0"/>
+        <v>2024</v>
+      </c>
+      <c r="M6">
+        <f t="shared" si="1"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A7" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="D7" s="14" t="s">
+        <v>47</v>
+      </c>
+      <c r="F7" s="11">
+        <v>81223400</v>
+      </c>
+      <c r="G7" s="11">
+        <v>81223400</v>
+      </c>
+      <c r="K7" s="32">
+        <v>45573</v>
+      </c>
+      <c r="L7">
+        <f t="shared" si="0"/>
+        <v>2024</v>
+      </c>
+      <c r="M7">
+        <f t="shared" si="1"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A8" s="19" t="s">
+        <v>51</v>
+      </c>
+      <c r="D8" s="19" t="s">
+        <v>52</v>
+      </c>
+      <c r="F8" s="20">
+        <v>620027595</v>
+      </c>
+      <c r="G8" s="20">
+        <v>620027595</v>
+      </c>
+      <c r="K8" s="31">
+        <v>45642</v>
+      </c>
+      <c r="L8">
+        <f t="shared" si="0"/>
+        <v>2024</v>
+      </c>
+      <c r="M8">
+        <f t="shared" si="1"/>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A9" s="14" t="s">
+        <v>56</v>
+      </c>
+      <c r="D9" s="14" t="s">
+        <v>57</v>
+      </c>
+      <c r="F9" s="11">
+        <v>26902449</v>
+      </c>
+      <c r="G9" s="11">
+        <v>26902449</v>
+      </c>
+      <c r="K9" s="32">
+        <v>45597</v>
+      </c>
+      <c r="L9">
+        <f t="shared" si="0"/>
+        <v>2024</v>
+      </c>
+      <c r="M9">
+        <f t="shared" si="1"/>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A10" s="72" t="s">
+        <v>59</v>
+      </c>
+      <c r="D10" s="72" t="s">
+        <v>60</v>
+      </c>
+      <c r="F10" s="75">
+        <v>73268018</v>
+      </c>
+      <c r="G10" s="75">
+        <v>73268018</v>
+      </c>
+      <c r="K10" s="71">
+        <v>45569</v>
+      </c>
+      <c r="L10">
+        <f t="shared" si="0"/>
+        <v>2024</v>
+      </c>
+      <c r="M10">
+        <f t="shared" si="1"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A11" s="14" t="s">
+        <v>64</v>
+      </c>
+      <c r="D11" s="14">
+        <v>5269803</v>
+      </c>
+      <c r="F11" s="11">
+        <v>65541486</v>
+      </c>
+      <c r="G11" s="11">
+        <v>65541486</v>
+      </c>
+      <c r="K11" s="32">
+        <v>45615</v>
+      </c>
+      <c r="L11">
+        <f t="shared" si="0"/>
+        <v>2024</v>
+      </c>
+      <c r="M11">
+        <f t="shared" si="1"/>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A12" s="72" t="s">
+        <v>67</v>
+      </c>
+      <c r="D12" s="72">
+        <v>37082297</v>
+      </c>
+      <c r="F12" s="75">
+        <f>57526407+2750000</f>
+        <v>60276407</v>
+      </c>
+      <c r="G12" s="75">
+        <f>57526407+2750000</f>
+        <v>60276407</v>
+      </c>
+      <c r="K12" s="71">
+        <v>45334</v>
+      </c>
+      <c r="L12">
+        <f t="shared" si="0"/>
+        <v>2024</v>
+      </c>
+      <c r="M12">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A13" s="18" t="s">
+        <v>70</v>
+      </c>
+      <c r="D13" s="19" t="s">
+        <v>71</v>
+      </c>
+      <c r="F13" s="20">
+        <v>239832910</v>
+      </c>
+      <c r="G13" s="20">
+        <v>239832910</v>
+      </c>
+      <c r="K13" s="31">
+        <v>45639</v>
+      </c>
+      <c r="L13">
+        <f t="shared" si="0"/>
+        <v>2024</v>
+      </c>
+      <c r="M13">
+        <f t="shared" si="1"/>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A14" s="38" t="s">
+        <v>75</v>
+      </c>
+      <c r="D14" s="36" t="s">
+        <v>76</v>
+      </c>
+      <c r="F14" s="39">
+        <v>279034822</v>
+      </c>
+      <c r="G14" s="39">
+        <v>279034822</v>
+      </c>
+      <c r="K14" s="35">
+        <v>45602</v>
+      </c>
+      <c r="L14">
+        <f t="shared" si="0"/>
+        <v>2024</v>
+      </c>
+      <c r="M14">
+        <f t="shared" si="1"/>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A15" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="D15" s="3">
+        <v>12957938</v>
+      </c>
+      <c r="F15" s="4">
+        <v>77736480</v>
+      </c>
+      <c r="G15" s="4">
+        <v>77736480</v>
+      </c>
+      <c r="K15" s="33">
+        <v>45649</v>
+      </c>
+      <c r="L15">
+        <f t="shared" si="0"/>
+        <v>2024</v>
+      </c>
+      <c r="M15">
+        <f t="shared" si="1"/>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A16" s="38" t="s">
+        <v>83</v>
+      </c>
+      <c r="D16" s="36" t="s">
+        <v>84</v>
+      </c>
+      <c r="F16" s="39">
+        <v>62633204</v>
+      </c>
+      <c r="G16" s="39">
+        <v>62633204</v>
+      </c>
+      <c r="K16" s="35">
+        <v>45652</v>
+      </c>
+      <c r="L16">
+        <f t="shared" si="0"/>
+        <v>2024</v>
+      </c>
+      <c r="M16">
+        <f t="shared" si="1"/>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A17" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="D17" s="3">
+        <v>16359436</v>
+      </c>
+      <c r="F17" s="4">
+        <v>252823862</v>
+      </c>
+      <c r="G17" s="4">
+        <v>252823862</v>
+      </c>
+      <c r="K17" s="33">
+        <v>45643</v>
+      </c>
+      <c r="L17">
+        <f t="shared" si="0"/>
+        <v>2024</v>
+      </c>
+      <c r="M17">
+        <f t="shared" si="1"/>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A18" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="D18" s="3">
+        <v>1144055891</v>
+      </c>
+      <c r="F18" s="4">
+        <v>28500000</v>
+      </c>
+      <c r="G18" s="4">
+        <v>28500000</v>
+      </c>
+      <c r="K18" s="33">
+        <v>45326</v>
+      </c>
+      <c r="L18">
+        <f t="shared" si="0"/>
+        <v>2024</v>
+      </c>
+      <c r="M18">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A19" s="95" t="s">
+        <v>95</v>
+      </c>
+      <c r="D19" s="108" t="s">
+        <v>96</v>
+      </c>
+      <c r="F19" s="97">
+        <v>212400000</v>
+      </c>
+      <c r="G19" s="97">
+        <v>212400000</v>
+      </c>
+      <c r="K19" s="94">
+        <v>45688</v>
+      </c>
+      <c r="L19">
+        <f t="shared" si="0"/>
+        <v>2025</v>
+      </c>
+      <c r="M19">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A20" s="79" t="s">
+        <v>99</v>
+      </c>
+      <c r="D20" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="F20" s="48">
+        <v>149513940</v>
+      </c>
+      <c r="G20" s="48">
+        <v>149513940</v>
+      </c>
+      <c r="K20" s="33">
+        <v>45743</v>
+      </c>
+      <c r="L20">
+        <f t="shared" si="0"/>
+        <v>2025</v>
+      </c>
+      <c r="M20">
+        <f t="shared" si="1"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A21" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="D21" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="F21" s="4">
+        <v>50550000</v>
+      </c>
+      <c r="G21" s="4">
+        <v>50550000</v>
+      </c>
+      <c r="K21" s="33">
+        <v>45743</v>
+      </c>
+      <c r="L21">
+        <f t="shared" si="0"/>
+        <v>2025</v>
+      </c>
+      <c r="M21">
+        <f t="shared" si="1"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A22" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="D22" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="F22" s="4">
+        <v>65000000</v>
+      </c>
+      <c r="G22" s="4">
+        <v>65000000</v>
+      </c>
+      <c r="K22" s="33">
+        <v>45763</v>
+      </c>
+      <c r="L22">
+        <f t="shared" si="0"/>
+        <v>2025</v>
+      </c>
+      <c r="M22">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A23" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="D23" s="3" t="s">
+        <v>116</v>
+      </c>
+      <c r="F23" s="4">
+        <v>106183000</v>
+      </c>
+      <c r="G23" s="4">
+        <v>106183000</v>
+      </c>
+      <c r="K23" s="45">
+        <v>45771</v>
+      </c>
+      <c r="L23">
+        <f t="shared" si="0"/>
+        <v>2025</v>
+      </c>
+      <c r="M23">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A24" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="D24" s="3" t="s">
+        <v>121</v>
+      </c>
+      <c r="F24" s="4">
+        <f>363610000+12000000+11006866</f>
+        <v>386616866</v>
+      </c>
+      <c r="G24" s="4">
+        <f>363610000+12000000+11006866</f>
+        <v>386616866</v>
+      </c>
+      <c r="K24" s="45">
+        <v>45797</v>
+      </c>
+      <c r="L24">
+        <f t="shared" si="0"/>
+        <v>2025</v>
+      </c>
+      <c r="M24">
+        <f t="shared" si="1"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A25" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="D25" s="3"/>
+      <c r="F25" s="4">
+        <v>669683741</v>
+      </c>
+      <c r="G25" s="4">
+        <v>669683741</v>
+      </c>
+      <c r="K25" s="45">
+        <v>45812</v>
+      </c>
+      <c r="L25">
+        <f t="shared" si="0"/>
+        <v>2025</v>
+      </c>
+      <c r="M25">
+        <f t="shared" si="1"/>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A26" s="131"/>
+      <c r="F26" s="4">
+        <v>32528526</v>
+      </c>
+      <c r="G26" s="4">
+        <v>32528526</v>
+      </c>
+      <c r="K26" s="45">
+        <v>45799</v>
+      </c>
+      <c r="L26">
+        <f t="shared" si="0"/>
+        <v>2025</v>
+      </c>
+      <c r="M26">
+        <f t="shared" si="1"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="27" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="F27" s="84"/>
+      <c r="G27" s="84"/>
+      <c r="K27" s="83"/>
+    </row>
+    <row r="29" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="G29" s="78">
+        <f>+SUM(G2:G26)</f>
+        <v>5405164720</v>
+      </c>
+    </row>
+    <row r="30" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="G30" s="78"/>
+    </row>
+    <row r="31" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="G31" s="78"/>
+    </row>
+    <row r="32" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="G32" s="78"/>
+    </row>
+    <row r="34" spans="7:7" x14ac:dyDescent="0.4">
+      <c r="G34" s="51"/>
+    </row>
+    <row r="37" spans="7:7" x14ac:dyDescent="0.4">
+      <c r="G37" s="51"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
+</worksheet>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <lcf76f155ced4ddcb4097134ff3c332f xmlns="e3263d6f-78a9-49ff-a5c9-96a22419e135">
@@ -3140,7 +3976,7 @@
 </p:properties>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x0101001A7F3C48C0DABA4BA49C1CE4049E40D3" ma:contentTypeVersion="16" ma:contentTypeDescription="Crear nuevo documento." ma:contentTypeScope="" ma:versionID="7f2be9710b812530dae8d902f02f3472">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="e3263d6f-78a9-49ff-a5c9-96a22419e135" xmlns:ns3="4c10c0ed-67ef-486e-8cdf-49cb961eb332" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="b2fb31d5ed747bfbc71c86180fe9a01c" ns2:_="" ns3:_="">
     <xsd:import namespace="e3263d6f-78a9-49ff-a5c9-96a22419e135"/>
@@ -3381,14 +4217,49 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3DE83D3E-89D2-4B0D-8EE2-F587AD043CE5}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F7BA6DB3-7253-4AE3-8B9E-B32F49E35C82}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="e3263d6f-78a9-49ff-a5c9-96a22419e135"/>
+    <ds:schemaRef ds:uri="4c10c0ed-67ef-486e-8cdf-49cb961eb332"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F7BA6DB3-7253-4AE3-8B9E-B32F49E35C82}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B1F6CDC0-A067-41BD-9AE3-B17D6DFDDF6B}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="e3263d6f-78a9-49ff-a5c9-96a22419e135"/>
+    <ds:schemaRef ds:uri="4c10c0ed-67ef-486e-8cdf-49cb961eb332"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B1F6CDC0-A067-41BD-9AE3-B17D6DFDDF6B}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3DE83D3E-89D2-4B0D-8EE2-F587AD043CE5}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>